<commit_message>
improve documentation, add a number of user-styles, closes #33
</commit_message>
<xml_diff>
--- a/documentation/Example files/contraception.xlsx
+++ b/documentation/Example files/contraception.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>list_name</t>
   </si>
   <si>
-    <t>skipif</t>
-  </si>
-  <si>
     <t>## Ihre Verhütung
 Nun stellen wir Ihnen einige Fragen zu Ihrer Verhütung.</t>
   </si>
@@ -1255,15 +1252,6 @@
     <t>select other_hormonal</t>
   </si>
   <si>
-    <t>contraception$pill != 'other'</t>
-  </si>
-  <si>
-    <t>! stringr::str_detect(contraception$contraceptives, 'contraceptive_pill')</t>
-  </si>
-  <si>
-    <t>! stringr::str_detect(contraception$contraceptives, 'other_hormonal')</t>
-  </si>
-  <si>
     <t>Welches hormonelle Verhütungsmittel benutzen Sie?</t>
   </si>
   <si>
@@ -1295,13 +1283,25 @@
   </si>
   <si>
     <t>Hormonspirale</t>
+  </si>
+  <si>
+    <t>showif</t>
+  </si>
+  <si>
+    <t>stringr::str_detect(contraception$contraceptives, 'contraceptive_pill')</t>
+  </si>
+  <si>
+    <t>stringr::str_detect(contraception$contraceptives, 'other_hormonal')</t>
+  </si>
+  <si>
+    <t>contraception$pill == 'other'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1383,6 +1383,22 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1401,8 +1417,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1447,7 +1465,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1780,8 +1800,8 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1816,7 +1836,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>10</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45">
@@ -1827,78 +1847,78 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="B3" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="C4" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="10" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="B5" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45">
       <c r="B6" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>413</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45">
@@ -1906,101 +1926,101 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="105">
       <c r="B10" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
       <c r="B11" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="120">
       <c r="B12" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="150">
       <c r="B13" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2076,44 +2096,44 @@
         <v>7</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>233</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>234</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>239</v>
-      </c>
       <c r="N1" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>334</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>335</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -2129,43 +2149,43 @@
     </row>
     <row r="3" spans="1:14">
       <c r="B3" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="21">
         <v>28</v>
       </c>
       <c r="H3" s="21"/>
       <c r="K3" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="M3" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="M3" s="21" t="s">
-        <v>231</v>
-      </c>
       <c r="N3" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14">
         <v>21</v>
@@ -2179,30 +2199,30 @@
         <v>420</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="16">
         <v>3000</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="14">
         <v>24</v>
@@ -2216,30 +2236,30 @@
         <v>360</v>
       </c>
       <c r="K5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="14" t="s">
-        <v>21</v>
-      </c>
       <c r="N5" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="B6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="14">
         <v>21</v>
@@ -2253,30 +2273,30 @@
         <v>420</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="14" t="s">
-        <v>30</v>
-      </c>
       <c r="N6" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="B7" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="19">
         <v>21</v>
@@ -2290,30 +2310,30 @@
         <v>735</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L7" s="20">
         <v>2000</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="14">
         <v>21</v>
@@ -2327,30 +2347,30 @@
         <v>630</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L8" s="16">
         <v>2000</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="14">
         <v>21</v>
@@ -2364,30 +2384,30 @@
         <v>630</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L9" s="16">
         <v>2000</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="19">
         <v>21</v>
@@ -2401,30 +2421,30 @@
         <v>735</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L10" s="20">
         <v>2000</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>80</v>
-      </c>
       <c r="E11" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="14">
         <v>21</v>
@@ -2438,30 +2458,30 @@
         <v>630</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L11" s="16">
         <v>2000</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="E12" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="14">
         <v>21</v>
@@ -2475,30 +2495,30 @@
         <v>630</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L12" s="16">
         <v>2000</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>164</v>
       </c>
       <c r="F13" s="14">
         <v>7</v>
@@ -2508,36 +2528,36 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J13" s="14">
         <v>730</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="E14" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="14">
         <v>21</v>
@@ -2551,57 +2571,57 @@
         <v>630</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L14" s="16">
         <v>2000</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15" s="21">
         <v>28</v>
       </c>
       <c r="H15" s="21"/>
       <c r="K15" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="L15" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>223</v>
-      </c>
       <c r="N15" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="14">
         <v>21</v>
@@ -2615,30 +2635,30 @@
         <v>630</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L16" s="16">
         <v>2000</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>173</v>
-      </c>
       <c r="E17" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="14">
         <v>21</v>
@@ -2652,30 +2672,30 @@
         <v>735</v>
       </c>
       <c r="K17" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="L17" s="14" t="s">
-        <v>175</v>
-      </c>
       <c r="M17" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>177</v>
-      </c>
       <c r="E18" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="19">
         <v>21</v>
@@ -2689,30 +2709,30 @@
         <v>735</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L18" s="20">
         <v>2000</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="14">
         <v>21</v>
@@ -2726,57 +2746,57 @@
         <v>630</v>
       </c>
       <c r="K19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="M19" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F20" s="21">
         <v>28</v>
       </c>
       <c r="H20" s="21"/>
       <c r="K20" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>180</v>
-      </c>
       <c r="E21" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="19">
         <v>21</v>
@@ -2790,30 +2810,30 @@
         <v>735</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L21" s="20">
         <v>2000</v>
       </c>
       <c r="M21" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>183</v>
-      </c>
       <c r="E22" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22" s="19">
         <v>21</v>
@@ -2827,57 +2847,57 @@
         <v>735</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L22" s="20">
         <v>2000</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="21">
         <v>28</v>
       </c>
       <c r="H23" s="21"/>
       <c r="K23" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24" s="14">
         <v>24</v>
@@ -2891,30 +2911,30 @@
         <v>480</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L24" s="16">
         <v>3000</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>32</v>
-      </c>
       <c r="E25" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F25" s="14">
         <v>21</v>
@@ -2928,30 +2948,30 @@
         <v>420</v>
       </c>
       <c r="K25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="M25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M25" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="N25" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F26" s="14">
         <v>21</v>
@@ -2965,30 +2985,30 @@
         <v>630</v>
       </c>
       <c r="K26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="M26" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="N26" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" s="19">
         <v>21</v>
@@ -3002,30 +3022,30 @@
         <v>735</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L27" s="20">
         <v>2000</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="14">
         <v>21</v>
@@ -3039,30 +3059,30 @@
         <v>630</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L28" s="16">
         <v>2000</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>188</v>
-      </c>
       <c r="E29" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" s="19">
         <v>21</v>
@@ -3076,30 +3096,30 @@
         <v>735</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L29" s="20">
         <v>2000</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="E30" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" s="14">
         <v>21</v>
@@ -3113,30 +3133,30 @@
         <v>420</v>
       </c>
       <c r="K30" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L30" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M30" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" s="14">
         <v>21</v>
@@ -3150,30 +3170,30 @@
         <v>630</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L31" s="16">
         <v>2000</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="E32" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" s="14">
         <v>21</v>
@@ -3187,30 +3207,30 @@
         <v>420</v>
       </c>
       <c r="K32" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="M32" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M32" s="14" t="s">
-        <v>30</v>
-      </c>
       <c r="N32" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" s="14">
         <v>21</v>
@@ -3224,30 +3244,30 @@
         <v>630</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M33" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N33" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="2:14">
       <c r="B34" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F34" s="14">
         <v>21</v>
@@ -3261,30 +3281,30 @@
         <v>420</v>
       </c>
       <c r="K34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L34" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="M34" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M34" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="N34" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="2:14">
       <c r="B35" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F35" s="14">
         <v>21</v>
@@ -3298,30 +3318,30 @@
         <v>630</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M35" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N35" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="2:14">
       <c r="B36" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C36" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="E36" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F36" s="14">
         <v>21</v>
@@ -3335,30 +3355,30 @@
         <v>630</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M36" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N36" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="E37" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F37" s="14">
         <v>21</v>
@@ -3372,30 +3392,30 @@
         <v>420</v>
       </c>
       <c r="K37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L37" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M37" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N37" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" spans="2:14">
       <c r="B38" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F38" s="14">
         <v>21</v>
@@ -3409,30 +3429,30 @@
         <v>630</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N38" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="2:14">
       <c r="B39" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F39" s="14">
         <v>21</v>
@@ -3446,30 +3466,30 @@
         <v>630</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L39" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M39" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="M39" s="14" t="s">
-        <v>108</v>
-      </c>
       <c r="N39" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="2:14">
       <c r="B40" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F40" s="14">
         <v>21</v>
@@ -3483,30 +3503,30 @@
         <v>420</v>
       </c>
       <c r="K40" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L40" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="M40" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N40" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="2:14">
       <c r="B41" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F41" s="14">
         <v>21</v>
@@ -3520,30 +3540,30 @@
         <v>1050</v>
       </c>
       <c r="K41" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N41" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" spans="2:14">
       <c r="B42" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C42" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="E42" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F42" s="14">
         <v>21</v>
@@ -3557,30 +3577,30 @@
         <v>420</v>
       </c>
       <c r="K42" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L42" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M42" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N42" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" s="19">
         <v>21</v>
@@ -3594,57 +3614,57 @@
         <v>735</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L43" s="20">
         <v>2000</v>
       </c>
       <c r="M43" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N43" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F44" s="21">
         <v>28</v>
       </c>
       <c r="H44" s="21"/>
       <c r="K44" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L44" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M44" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N44" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>193</v>
-      </c>
       <c r="E45" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" s="19">
         <v>21</v>
@@ -3658,30 +3678,30 @@
         <v>735</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L45" s="20">
         <v>2000</v>
       </c>
       <c r="M45" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N45" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="2:14">
       <c r="B46" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" s="14">
         <v>21</v>
@@ -3695,30 +3715,30 @@
         <v>420</v>
       </c>
       <c r="K46" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L46" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L46" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="M46" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N46" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="2:14">
       <c r="B47" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" s="14">
         <v>21</v>
@@ -3732,30 +3752,30 @@
         <v>630</v>
       </c>
       <c r="K47" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L47" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="M47" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N47" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="2:14">
       <c r="B48" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>56</v>
-      </c>
       <c r="E48" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" s="14">
         <v>21</v>
@@ -3769,30 +3789,30 @@
         <v>420</v>
       </c>
       <c r="K48" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L48" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M48" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N48" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="2:14">
       <c r="B49" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F49" s="14">
         <v>21</v>
@@ -3806,30 +3826,30 @@
         <v>420</v>
       </c>
       <c r="K49" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L49" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M49" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" spans="2:14">
       <c r="B50" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C50" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>111</v>
-      </c>
       <c r="E50" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F50" s="14">
         <v>21</v>
@@ -3843,30 +3863,30 @@
         <v>630</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L50" s="16">
         <v>2000</v>
       </c>
       <c r="M50" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N50" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F51" s="14">
         <v>21</v>
@@ -3880,30 +3900,30 @@
         <v>630</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L51" s="16">
         <v>2000</v>
       </c>
       <c r="M51" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N51" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="2:14">
       <c r="B52" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C52" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="E52" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F52" s="14">
         <v>21</v>
@@ -3917,30 +3937,30 @@
         <v>420</v>
       </c>
       <c r="K52" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L52" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L52" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="M52" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N52" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="53" spans="2:14">
       <c r="B53" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C53" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="E53" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F53" s="14">
         <v>21</v>
@@ -3954,30 +3974,30 @@
         <v>420</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L53" s="16">
         <v>3000</v>
       </c>
       <c r="M53" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N53" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F54" s="14">
         <v>21</v>
@@ -3991,30 +4011,30 @@
         <v>630</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L54" s="16">
         <v>3000</v>
       </c>
       <c r="M54" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N54" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="2:14">
       <c r="B55" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F55" s="14">
         <v>21</v>
@@ -4028,30 +4048,30 @@
         <v>630</v>
       </c>
       <c r="K55" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L55" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="M55" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N55" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56" spans="2:14">
       <c r="B56" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F56" s="14">
         <v>21</v>
@@ -4065,30 +4085,30 @@
         <v>630</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L56" s="16">
         <v>2000</v>
       </c>
       <c r="M56" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N56" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="57" spans="2:14">
       <c r="B57" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F57" s="14">
         <v>21</v>
@@ -4102,30 +4122,30 @@
         <v>630</v>
       </c>
       <c r="K57" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L57" s="16">
         <v>2000</v>
       </c>
       <c r="M57" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N57" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58" spans="2:14">
       <c r="B58" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F58" s="14">
         <v>21</v>
@@ -4139,57 +4159,57 @@
         <v>630</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M58" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N58" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59" spans="2:14">
       <c r="B59" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F59" s="21">
         <v>35</v>
       </c>
       <c r="H59" s="21"/>
       <c r="K59" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="L59" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="L59" s="21" t="s">
+      <c r="M59" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="M59" s="21" t="s">
-        <v>231</v>
-      </c>
       <c r="N59" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="2:14">
       <c r="B60" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C60" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D60" s="13" t="s">
-        <v>124</v>
-      </c>
       <c r="E60" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F60" s="14">
         <v>21</v>
@@ -4203,30 +4223,30 @@
         <v>630</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L60" s="16">
         <v>2000</v>
       </c>
       <c r="M60" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N60" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="2:14">
       <c r="B61" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F61" s="14">
         <v>21</v>
@@ -4240,30 +4260,30 @@
         <v>630</v>
       </c>
       <c r="K61" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L61" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="M61" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="M61" s="14" t="s">
-        <v>128</v>
-      </c>
       <c r="N61" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="2:14">
       <c r="B62" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F62" s="14">
         <v>21</v>
@@ -4277,30 +4297,30 @@
         <v>420</v>
       </c>
       <c r="K62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L62" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M62" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N62" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="2:14">
       <c r="B63" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F63" s="14">
         <v>21</v>
@@ -4314,30 +4334,30 @@
         <v>630</v>
       </c>
       <c r="K63" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L63" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M63" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N63" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="2:14">
       <c r="B64" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C64" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="E64" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F64" s="14">
         <v>21</v>
@@ -4351,30 +4371,30 @@
         <v>420</v>
       </c>
       <c r="K64" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L64" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L64" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="M64" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N64" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="2:14">
       <c r="B65" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="14">
         <v>21</v>
@@ -4388,30 +4408,30 @@
         <v>630</v>
       </c>
       <c r="K65" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L65" s="16">
         <v>2000</v>
       </c>
       <c r="M65" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N65" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66" spans="2:14">
       <c r="B66" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C66" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D66" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="E66" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F66" s="14">
         <v>21</v>
@@ -4425,30 +4445,30 @@
         <v>630</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L66" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M66" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N66" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="2:14">
       <c r="B67" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C67" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D67" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="D67" s="18" t="s">
-        <v>195</v>
-      </c>
       <c r="E67" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F67" s="19">
         <v>21</v>
@@ -4462,30 +4482,30 @@
         <v>735</v>
       </c>
       <c r="K67" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L67" s="20">
         <v>2000</v>
       </c>
       <c r="M67" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N67" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="68" spans="2:14">
       <c r="B68" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C68" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>208</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>209</v>
       </c>
       <c r="F68" s="14">
         <v>11</v>
@@ -4495,36 +4515,36 @@
       </c>
       <c r="H68" s="15"/>
       <c r="I68" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J68" s="14">
         <v>1150</v>
       </c>
       <c r="K68" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L68" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="M68" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="M68" s="14" t="s">
-        <v>212</v>
-      </c>
       <c r="N68" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="69" spans="2:14">
       <c r="B69" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F69" s="14">
         <v>6</v>
@@ -4536,36 +4556,36 @@
         <v>10</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J69" s="14">
         <v>680</v>
       </c>
       <c r="K69" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L69" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="M69" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="M69" s="14" t="s">
-        <v>155</v>
-      </c>
       <c r="N69" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="70" spans="2:14">
       <c r="B70" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C70" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F70" s="14">
         <v>7</v>
@@ -4577,36 +4597,36 @@
         <v>7</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J70" s="14">
         <v>665</v>
       </c>
       <c r="K70" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L70" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="M70" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="M70" s="14" t="s">
-        <v>151</v>
-      </c>
       <c r="N70" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="71" spans="2:14">
       <c r="B71" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F71" s="14">
         <v>21</v>
@@ -4620,30 +4640,30 @@
         <v>630</v>
       </c>
       <c r="K71" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L71" s="16">
         <v>3000</v>
       </c>
       <c r="M71" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N71" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="72" spans="2:14">
       <c r="B72" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C72" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="E72" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F72" s="14">
         <v>21</v>
@@ -4657,30 +4677,30 @@
         <v>630</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L72" s="16">
         <v>2000</v>
       </c>
       <c r="M72" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N72" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="2:14">
       <c r="B73" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F73" s="14">
         <v>7</v>
@@ -4692,36 +4712,36 @@
         <v>7</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J73" s="14">
         <v>735</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L73" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M73" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="M73" s="14" t="s">
-        <v>199</v>
-      </c>
       <c r="N73" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="74" spans="2:14">
       <c r="B74" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C74" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>214</v>
       </c>
       <c r="F74" s="14">
         <v>26</v>
@@ -4739,30 +4759,30 @@
         <v>3</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L74" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="M74" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="M74" s="14" t="s">
-        <v>216</v>
-      </c>
       <c r="N74" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="75" spans="2:14">
       <c r="B75" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F75" s="14">
         <v>7</v>
@@ -4774,36 +4794,36 @@
         <v>5</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J75" s="14">
         <v>735</v>
       </c>
       <c r="K75" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L75" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="M75" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="M75" s="14" t="s">
-        <v>202</v>
-      </c>
       <c r="N75" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="2:14">
       <c r="B76" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F76" s="14">
         <v>6</v>
@@ -4815,36 +4835,36 @@
         <v>10</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J76" s="14">
         <v>680</v>
       </c>
       <c r="K76" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L76" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="M76" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="M76" s="14" t="s">
-        <v>158</v>
-      </c>
       <c r="N76" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="77" spans="2:14">
       <c r="B77" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F77" s="14">
         <v>7</v>
@@ -4856,36 +4876,36 @@
         <v>7</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J77" s="14">
         <v>735</v>
       </c>
       <c r="K77" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L77" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M77" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="M77" s="14" t="s">
-        <v>205</v>
-      </c>
       <c r="N77" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="78" spans="2:14">
       <c r="B78" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F78" s="14">
         <v>6</v>
@@ -4897,36 +4917,36 @@
         <v>10</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J78" s="14">
         <v>680</v>
       </c>
       <c r="K78" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L78" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M78" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N78" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="79" spans="2:14">
       <c r="B79" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F79" s="14">
         <v>6</v>
@@ -4938,36 +4958,36 @@
         <v>9</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J79" s="14">
         <v>680</v>
       </c>
       <c r="K79" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L79" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M79" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N79" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="80" spans="2:14">
       <c r="B80" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F80" s="14">
         <v>21</v>
@@ -4981,30 +5001,30 @@
         <v>630</v>
       </c>
       <c r="K80" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L80" s="16">
         <v>2000</v>
       </c>
       <c r="M80" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N80" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="81" spans="1:14">
       <c r="B81" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C81" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D81" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D81" s="13" t="s">
-        <v>141</v>
-      </c>
       <c r="E81" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F81" s="14">
         <v>21</v>
@@ -5018,30 +5038,30 @@
         <v>630</v>
       </c>
       <c r="K81" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L81" s="16">
         <v>2000</v>
       </c>
       <c r="M81" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N81" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:14">
       <c r="B82" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F82" s="14">
         <v>21</v>
@@ -5055,30 +5075,30 @@
         <v>630</v>
       </c>
       <c r="K82" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L82" s="16">
         <v>2000</v>
       </c>
       <c r="M82" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N82" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:14">
       <c r="B83" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F83" s="14">
         <v>21</v>
@@ -5092,30 +5112,30 @@
         <v>630</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L83" s="16">
         <v>2000</v>
       </c>
       <c r="M83" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N83" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="84" spans="1:14">
       <c r="B84" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F84" s="14">
         <v>21</v>
@@ -5129,30 +5149,30 @@
         <v>630</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L84" s="16">
         <v>3000</v>
       </c>
       <c r="M84" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N84" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:14">
       <c r="B85" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F85" s="14">
         <v>21</v>
@@ -5166,30 +5186,30 @@
         <v>420</v>
       </c>
       <c r="K85" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L85" s="16">
         <v>3000</v>
       </c>
       <c r="M85" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N85" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:14">
       <c r="B86" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F86" s="14">
         <v>24</v>
@@ -5203,30 +5223,30 @@
         <v>480</v>
       </c>
       <c r="K86" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L86" s="16">
         <v>3000</v>
       </c>
       <c r="M86" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N86" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" spans="1:14">
       <c r="B87" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C87" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D87" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D87" s="13" t="s">
-        <v>218</v>
-      </c>
       <c r="E87" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F87" s="14">
         <v>24</v>
@@ -5244,59 +5264,59 @@
         <v>3</v>
       </c>
       <c r="K87" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L87" s="16">
         <v>2500</v>
       </c>
       <c r="M87" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N87" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="90" spans="1:14">
       <c r="B90" s="12" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="91" spans="1:14">
       <c r="B91" s="12" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="B92" s="12" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="B93" s="12" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -5305,232 +5325,232 @@
     </row>
     <row r="96" spans="1:14">
       <c r="A96" t="s">
+        <v>348</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C96" s="14" t="s">
         <v>349</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="B97" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="B98" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="B99" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="B100" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="B101" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="B102" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C102" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="B103" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="B104" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C104" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="B106" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="B107" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>364</v>
+      </c>
+      <c r="B110" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="C110" s="14" t="s">
         <v>366</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="B111" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C112" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="C114" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="C114" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="C115" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C116" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="C116" s="14" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="117" spans="2:3">
       <c r="B117" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="C117" s="14" t="s">
         <v>383</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="118" spans="2:3">
       <c r="B118" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="C118" s="14" t="s">
         <v>368</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="119" spans="2:3">
       <c r="B119" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C119" s="14" t="s">
         <v>385</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="120" spans="2:3">
       <c r="B120" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C120" s="14" t="s">
         <v>387</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C121" s="14" t="s">
         <v>371</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="123" spans="2:3">
       <c r="B123" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C123" s="14" t="s">
         <v>390</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="124" spans="2:3">
       <c r="B124" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C124" s="14" t="s">
         <v>392</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="125" spans="2:3">
       <c r="B125" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C125" s="14" t="s">
         <v>394</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>